<commit_message>
fix: add survey results and iteration output
</commit_message>
<xml_diff>
--- a/originaloutput/Iteration_2.xlsx
+++ b/originaloutput/Iteration_2.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Desktop\Dev\CodePilot\originaloutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16A82D76-82EA-4AF6-89CA-9450AF3B13FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE649F3C-B147-4313-8BF4-E44E2748AF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{288DA7EC-22F0-4E17-B473-DAE653BDB1E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2 mit Codefehlern" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Iteration 2 ohne Codefehler" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>Wo</t>
   </si>
@@ -335,6 +335,101 @@
 • Überlege, ob du das Überlaufverhalten gezielt mit checked steuerst oder es dokumentierst.Stil- und Verständlichkeits­verbesserungen
 • Nutze bei einzeiligen Schleifen immer geschweifte Klammern – das erhöht die Lesbarkeit und verhindert spätere Fehler beim Einfügen weiterer Zeilen.
 • Du könntest statt der expliziten Schleife auch LINQ (nums.Select(n =&gt; n + 1).ToArray()) einsetzen, wenn du mehr auf Ausdruckskraft als auf maximale Performance setzt.</t>
+  </si>
+  <si>
+    <t>Hier ein paar gezielte Hinweise, ohne die komplette Lösung vorwegzunehmen:Mögliche Fehler/RisikenWas passiert, wenn nums null ist? Eine zusätzliche Prüfung (Argument-Validation) verhindert eine NullReferenceException.Könnten Überläufe bei extrem großen Werten auftreten? Im vorliegenden Wertebereich (±10⁹) ist int zwar sicher, aber ein Gedanke für allgemeineren Code.Nächster sinn­voller VerbesserungsschrittÜberlege, ob du statt der manuellen Schleife LINQ einsetzen möchtest. Das macht den Code kurz und ausdrucksstark, ist aber nicht in jedem Szenario performanter.Beispiel als Hinweis (kein vollständiges Rewrite!):
+return nums.Select(n =&gt; n + 1).ToArray();
+Stil- und Verständlichkeits­verbesserungenZieh in Betracht, den Methodenkörper als Expression-Bodied Member zu schreiben, wenn wirklich nur eine Zeile übrig bleibt.Achte auf einheitliche Einrückungen und Klammer­setzung – das erhöht die Lesbarkeit, besonders bei späteren Anpassungen.</t>
+  </si>
+  <si>
+    <t>Hier ein paar Punkte, die du noch verbessern kannst, ohne die Lösung vorwegzunehmen:Mögliche Fehler/Risiken
+– Was passiert, wenn der Aufrufer null übergibt? In der aktuellen Fassung würdest du eine NullReferenceException bekommen.
+– Bei sehr großen Werten könnte das Inkrement theoretisch zum Overflow führen (in deinem Anwendungsbereich aktuell unwahrscheinlich, aber im Idealfall im Blick behalten).Nächster sinnvoller Schritt
+– Füge eine Argument-Prüfung hinzu, z. B. if (nums == null) throw new ArgumentNullException(nameof(nums));.
+– Überlege, ob du statt der Schleife ein sprachfeatures wie LINQ (nums.Select(...)) oder Array.ConvertAll einsetzen möchtest, um den Code kürzer und deklarativer zu machen.Stil-/Verständlichkeitsverbesserungen
+– Auch bei einzelnen Zeilen in einer Schleife sollte man aus Konsistenzgründen immer geschweifte Klammern benutzen.
+– Du könntest die Methode als Expression-Bodied Member schreiben, um sie kompakter zu gestalten.Diese Schritte erhöhen Robustheit, Lesbarkeit und nutzen moderne C#-Features.</t>
+  </si>
+  <si>
+    <t>Hier ein paar Hinweise zur schrittweisen Verbesserung deines Codes:Mögliche Fehler oder RisikenWenn nums null ist, wirft deine Methode eine NullReferenceException. Auch wenn du davon ausgehst, dass immer ein Array reinkommt, lohnt sich ein kurzer Null-Check oder eine klare Fehlermeldung (ArgumentNullException).Nächster sinnvoller VerbesserungsschrittNutze LINQ für mehr Lesbarkeit und Kürze. Statt der klassischen Schleife könntest du schreiben:
+return nums.Select(n =&gt; n + 1).ToArray();
+So beschränkst du dich auf die Geschäftslogik („jeden Wert um 1 erhöhen“) und überlässt die Iteration dem Framework.Stil- und VerständlichkeitsverbesserungenBaue bei Schleifen immer geschweifte Klammern ein, auch wenn sie nur eine Zeile umfassen – das hilft, Fehler beim Hinzufügen von Code zu vermeiden.Erwäge aussagekräftigere Namen (z. B. original statt nums, wenn es die Lesbarkeit verbessert).Mach die Methode statisch, falls sie keinen Objektzustand nutzt:
+public static int[] IncrementArray(int[] nums) { … }</t>
+  </si>
+  <si>
+    <t>Hier ein paar kurze Hinweise zur Verbesserung deines Codes, ohne gleich die komplette Lösung vorwegzunehmen:Mögliche Fehler/Risiken
+– Null-Eingabe: Wenn nums null ist, wirft dein Code eine unhandliche NullReferenceException. Ein früher Guard-Check hilft hier.
+– Integer-Overflow: Wenn ein Wert in nums bei int.MaxValue liegt, führt +1 zu einem Überlauf (sofern nicht im checked-Kontext).Nächster sinnvoller Schritt
+– Füge einen Guard-Check hinzu:
+csharp if (nums == null) throw new ArgumentNullException(nameof(nums)); 
+– Entscheide, ob du Überlauf prüfen möchtest (z. B. checkedBlock oder manuelle Prüfung).Stil-/Verständlichkeits-Tipps
+– Verwende stets geschweifte Klammern { … } auch bei einzeiligen Schleifen, um Lesbarkeit und Wartbarkeit zu erhöhen.
+– Überlege, ob du für so einfache Transformationen nicht LINQ oder Array.ConvertAll nutzen möchtest, um den Code kompakter zu gestalten.Damit hast du eine solide Basis, um die Methode robust und gut lesbar zu machen.</t>
+  </si>
+  <si>
+    <t>Hier ein paar kurze Hinweise, ohne gleich die Komplett-Lösung vorwegzunehmen:Mögliche Fehler/RisikenWas passiert, wenn jemand nums als null übergibt?Bei sehr großen Werten (z.B. int.MaxValue) kann das Hochzählen einen Überlauf auslösen.Nächster sinn­voller VerbesserungsschrittFüge eine Argument­validierung hinzu (z.B. if (nums == null) throw new ArgumentNullException(...)).Überlege, ob du im überlauf-sensitiven Szenario ein checkedKontext oder zumindest einen Pre-Check auf int.MaxValue brauchst.Kleine Stil- und Verständlichkeits­verbesserungenNutze durchgängig geschweifte Klammern für Schleifen/Blöcke, auch wenn nur eine Zeile folgt.Ziehe var für lokale Variablen in Betracht, wenn der Typ klar ist.Für eine kompakte Variante könntest du später einmal mit LINQ experimentieren (z.B. nums.Select(n =&gt; n + 1).ToArray()), beachte aber den Overhead.Beispiel für Null-Check und Stil:public int[] IncrementArray(int[] nums)
+{ if (nums == null) throw new ArgumentNullException(nameof(nums)); var result = new int[nums.Length]; for (var i = 0; i &lt; nums.Length; i++) { checked { result[i] = nums[i] + 1; } } return result;
+}</t>
+  </si>
+  <si>
+    <t>Hier ein kurzer Hinweis zur Verbesserung – ohne die komplette Lösung vorwegzunehmen:Mögliche Fehler/Risiken
+– Null‐Eingabe: Was passiert, wenn nums null ist?
+– Integer‐Overflow: nums[i] könnte int.MaxValue sein und beim „+1“ überlaufen.Nächster sinnvoller Schritt
+– Füge eine Eingabeprüfung ein (z. B. auf null) und entscheide, wie du damit umgehen willst.
+– Überlege, ob du bei Bedarf in einem checked‐Block arbeitest, um Überläufe zu erkennen.Stil-/Verständlichkeits­verbesserungen
+– Klammern um den forBlock komplettieren, auch bei einzeiligen Schleifen, für bessere Lesbarkeit.
+– Erwäge den Einsatz von LINQ (nums.Select(x =&gt; x + 1).ToArray()) oder eines expression-bodied members für noch kompakteren Code.
+– Nutze im Methodenkörper ruhig var, wenn der Typ klar ist (z. B. var result = new int[nums.Length];).</t>
+  </si>
+  <si>
+    <t>Hier ein paar kurze Hinweise, wie du deinen Code weiter verbessern kannst:Mögliche Fehler/RisikenNull-Referenz: Wenn nums unerwartet null ist, gibt es eine Exception.Überlauf: Würdest du an einem Element int.MaxValue + 1 rechnen, käme es zum Wrap-around.Nächster sinnvoller SchrittÜberlege, ob du eine Eingangs-Validierung (z. B. auf null) brauchst oder in-place arbeitest, um Speicher zu sparen.Alternativ kannst du mit LINQ in einer Zeile transformieren:
+„nums.Select(x =&gt; x + 1).ToArray()“.Stil-/Verständlichkeits-VerbesserungenImmer geschweifte Klammern um Schleifen/Ifs setzen, auch bei nur einer Zeile.Einheitliche Einrückung und bei lokalen Variablen evtl. var verwenden.Methodensignatur als Expression‐Bodied Member:public int[] IncrementArray(int[] nums) =&gt; nums.Select(x =&gt; x + 1).ToArray();</t>
+  </si>
+  <si>
+    <t>Dein Code erfüllt die Aufgabe korrekt und ist gut lesbar.Du könntest Array.ConvertAll(nums, n =&gt; n + 1) oder LINQ (nums.Select(n =&gt; n + 1).ToArray()) einsetzen, um den Kern in eine Zeile zu packen.Für extrem große Arrays ließe sich auch Parallel.For nutzen, um die Arbeit auf mehrere Threads zu verteilen.In performancekritischen Szenarien bieten sich Span&lt;T&gt; oder SIMD-Vektorisierungen unter .NET Core an.</t>
+  </si>
+  <si>
+    <t>Dein Ansatz ist korrekt und durchläuft das Array in O(n), aber hier ein paar Denkanstöße zur Verbesserung:Du könntest auf eine separate Ergebnis-Array verzichten und stattdessen das übergebene Array direkt anpassen, wenn keine ursprüngliche Kopie benötigt wird.Mit LINQ ließe sich die Methode sehr knapp als return nums.Select(x =&gt; x + 1).ToArray(); schreiben und wäre zugleich gut lesbar.Für High-Performance-Szenarien könnte ein Span&lt;int&gt; oder Memory&lt;int&gt; helfen, um Zwischenspeicher zu vermeiden.</t>
+  </si>
+  <si>
+    <t>Dein Code ist funktional korrekt und übersichtlich, die Schleifenbedingung „i &lt; nums.Length“ passt.Du könntest stattdessen einmal LINQ einsetzen, z. B.
+return nums.Select(x =&gt; x + 1).ToArray();
+um die Logik als Ein-Zeiler auszudrücken.Wenn du Speicher sparen willst und das Original-Array nicht mehr benötigst, lässt sich auch direkt in-place hochzählen (ohne neues Array).</t>
+  </si>
+  <si>
+    <t>Dein Algorithmus ist bereits korrekt und durchläuft das Array in linearer Zeit (O(n)).
+• Du könntest mit LINQ etwas kompakter schreiben, etwa nums.Select(n =&gt; n + 1).ToArray().
+• Wenn keine Kopie nötig ist, ließe sich das Original-Array in-place anpassen und so Speicher sparen.
+• Eine expression-bodied Methode (=&gt;) steigert zusätzlich die Lesbarkeit.</t>
+  </si>
+  <si>
+    <t>Der Ansatz funktioniert einwandfrei und ist klar verständlich.
+Als Alternative könntest du LINQ nutzen, etwa mit nums.Select(n =&gt; n + 1).ToArray(), um die Schleife prägnanter auszudrücken.
+Ebenso wäre Array.ConvertAll(nums, n =&gt; n + 1) eine kompakte Möglichkeit.
+Falls dir Performance und Speicherfehler wichtig sind, lohnt sich ein Blick auf Span&lt;T&gt; für zero-allocation-Szenarien.</t>
+  </si>
+  <si>
+    <t>Dein Ansatz ist korrekt und durchläuft das Array in O(n), um jedes Element um 1 zu erhöhen.Mit LINQ ließe sich die Schleife kompakter ausdrücken, etwa über nums.Select(n =&gt; n + 1).ToArray().Bei sehr großen Arrays könnte man alternativ mit Span&lt;T&gt; oder einer In-Place-Operation experimentieren, um zusätzlichen Speicher zu sparen.Auch Array.ConvertAll(nums, n =&gt; n + 1) bietet eine eingebaute, gut lesbare Alternative.</t>
+  </si>
+  <si>
+    <t>Dein Code erfüllt die Aufgabe und ist schon recht klar strukturiert.
+Überlege, ob du die Zugriffe auf nums.Length vor der Schleife in einer lokalen Variable cachest – ein winziger Performance-Gewinn bei sehr großen Arrays.
+Alternativ könntest du mit LINQ etwa nums.Select(x =&gt; x + 1).ToArray() einsetzen, um den Code kürzer und deklarativer zu gestalten.
+Falls dir ein In-Place-Update genügt, könntest du auch direkt über nums iterieren und die Originalwerte überschreiben.</t>
+  </si>
+  <si>
+    <t>Dein Code ist bereits funktional korrekt und läuft in O(n) mit minimalem Speicher-Overhead.
+Als Alternative könntest du statt der manuellen Schleife auch LINQ verwenden, z. B.return nums.Select(x =&gt; x + 1).ToArray();
+Das macht den Code kompakter, wirkt aber intern ähnlich performant.</t>
+  </si>
+  <si>
+    <t>Dein Ansatz läuft bereits in O(n) und liefert korrekt für jedes Element eins drauf.Wenn eine In-Place-Änderung ausreicht, könntest du auf das neue Array verzichten und direkt in nums inkrementieren.Für dreizeilige Kürze und höhere Lesbarkeit eignet sich LINQ: nums.Select(n =&gt; n + 1).ToArray().Eine expression-bodied Method (public int[] IncrementArray(int[] nums) =&gt; nums.Select(n =&gt; n+1).ToArray();) macht den Code noch kompakter.</t>
+  </si>
+  <si>
+    <t>Der Code ist korrekt lauffähig und sehr übersichtlich.
+Um den Zugriff auf nums.Length in jeder Schleifeniteration zu vermeiden, könntest du den Wert einmal in einer lokalen Variable speichern.
+Alternativ lässt sich die Aufgabe noch kompakter mit Array.ConvertAll(nums, x =&gt; x + 1) oder LINQ (nums.Select(x =&gt; x + 1).ToArray()) lösen.
+Falls das Original-Array nicht erhalten bleiben muss, käme auch eine In-Place-Änderung mittels Span&lt;int&gt; oder direkter Schleifenmodifikation infrage.</t>
   </si>
 </sst>
 </file>
@@ -852,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4B7F67-FB07-4A26-AB31-C04B7B2DD11D}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:M5"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +1009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -996,7 +1091,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="375" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1091,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9734FD-0BE7-49B7-B293-8C08BE1F0E6A}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1163,34 +1258,34 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
@@ -1213,28 +1308,28 @@
         <v>67</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>